<commit_message>
2des pwbe aula07 add instrucoes
</commit_message>
<xml_diff>
--- a/2des/chamada.xlsx
+++ b/2des/chamada.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2022\2des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A467902-6E12-48F6-9883-68124FF353D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABA06BA-BD15-4B35-9557-6B25D91280BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="36">
   <si>
     <t>Aluno</t>
   </si>
@@ -520,8 +520,8 @@
   <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AT10" sqref="AT10"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL31" sqref="AL31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +939,9 @@
       <c r="AK3" t="s">
         <v>35</v>
       </c>
+      <c r="AL3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1052,6 +1055,9 @@
       <c r="AK4" t="s">
         <v>35</v>
       </c>
+      <c r="AL4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1165,6 +1171,9 @@
       <c r="AK5" t="s">
         <v>35</v>
       </c>
+      <c r="AL5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1278,6 +1287,9 @@
       <c r="AK6" t="s">
         <v>35</v>
       </c>
+      <c r="AL6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1391,6 +1403,9 @@
       <c r="AK7" t="s">
         <v>35</v>
       </c>
+      <c r="AL7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1504,6 +1519,9 @@
       <c r="AK8" t="s">
         <v>35</v>
       </c>
+      <c r="AL8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1617,6 +1635,9 @@
       <c r="AK9" t="s">
         <v>34</v>
       </c>
+      <c r="AL9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1730,6 +1751,9 @@
       <c r="AK10" t="s">
         <v>35</v>
       </c>
+      <c r="AL10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1843,6 +1867,9 @@
       <c r="AK11" t="s">
         <v>35</v>
       </c>
+      <c r="AL11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2042,6 +2069,9 @@
       <c r="AK13" t="s">
         <v>35</v>
       </c>
+      <c r="AL13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2155,6 +2185,9 @@
       <c r="AK14" t="s">
         <v>35</v>
       </c>
+      <c r="AL14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2268,6 +2301,9 @@
       <c r="AK15" t="s">
         <v>34</v>
       </c>
+      <c r="AL15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2381,8 +2417,11 @@
       <c r="AK16" t="s">
         <v>35</v>
       </c>
+      <c r="AL16" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2494,8 +2533,11 @@
       <c r="AK17" t="s">
         <v>35</v>
       </c>
+      <c r="AL17" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2607,8 +2649,11 @@
       <c r="AK18" t="s">
         <v>35</v>
       </c>
+      <c r="AL18" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2720,8 +2765,11 @@
       <c r="AK19" t="s">
         <v>35</v>
       </c>
+      <c r="AL19" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2833,8 +2881,11 @@
       <c r="AK20" t="s">
         <v>35</v>
       </c>
+      <c r="AL20" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2946,8 +2997,11 @@
       <c r="AK21" t="s">
         <v>35</v>
       </c>
+      <c r="AL21" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3059,8 +3113,11 @@
       <c r="AK22" t="s">
         <v>35</v>
       </c>
+      <c r="AL22" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3172,8 +3229,11 @@
       <c r="AK23" t="s">
         <v>35</v>
       </c>
+      <c r="AL23" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3285,8 +3345,11 @@
       <c r="AK24" t="s">
         <v>35</v>
       </c>
+      <c r="AL24" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3398,8 +3461,11 @@
       <c r="AK25" t="s">
         <v>35</v>
       </c>
+      <c r="AL25" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3511,8 +3577,11 @@
       <c r="AK26" t="s">
         <v>34</v>
       </c>
+      <c r="AL26" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3624,8 +3693,11 @@
       <c r="AK27" t="s">
         <v>35</v>
       </c>
+      <c r="AL27" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3737,8 +3809,11 @@
       <c r="AK28" t="s">
         <v>35</v>
       </c>
+      <c r="AL28" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3850,8 +3925,11 @@
       <c r="AK29" t="s">
         <v>35</v>
       </c>
+      <c r="AL29" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -3961,6 +4039,9 @@
         <v>35</v>
       </c>
       <c r="AK30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL30" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2DES BCD AULAS REORGANIZADAS
</commit_message>
<xml_diff>
--- a/2des/chamada.xlsx
+++ b/2des/chamada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2022\2des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9CF6C1-3791-4C55-8FA6-E05E4AC4CFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB5EC7-A0AF-4D07-8C58-3DE0C959B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="37">
   <si>
     <t>Aluno</t>
   </si>
@@ -522,7 +522,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BB24" sqref="BB24"/>
+      <selection pane="topRight" activeCell="AY27" sqref="AY27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,6 +1018,9 @@
       <c r="AX3" t="s">
         <v>35</v>
       </c>
+      <c r="AY3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1164,6 +1167,9 @@
       <c r="AX4" t="s">
         <v>35</v>
       </c>
+      <c r="AY4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1310,6 +1316,9 @@
       <c r="AX5" t="s">
         <v>35</v>
       </c>
+      <c r="AY5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1456,6 +1465,9 @@
       <c r="AX6" t="s">
         <v>35</v>
       </c>
+      <c r="AY6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1602,6 +1614,9 @@
       <c r="AX7" t="s">
         <v>34</v>
       </c>
+      <c r="AY7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1748,6 +1763,9 @@
       <c r="AX8" t="s">
         <v>35</v>
       </c>
+      <c r="AY8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1894,6 +1912,9 @@
       <c r="AX9" t="s">
         <v>35</v>
       </c>
+      <c r="AY9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2040,6 +2061,9 @@
       <c r="AX10" t="s">
         <v>35</v>
       </c>
+      <c r="AY10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2186,6 +2210,9 @@
       <c r="AX11" t="s">
         <v>35</v>
       </c>
+      <c r="AY11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2332,6 +2359,9 @@
       <c r="AX12" t="s">
         <v>35</v>
       </c>
+      <c r="AY12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2567,6 +2597,9 @@
       <c r="AX14" t="s">
         <v>35</v>
       </c>
+      <c r="AY14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2713,6 +2746,9 @@
       <c r="AX15" t="s">
         <v>35</v>
       </c>
+      <c r="AY15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2859,8 +2895,11 @@
       <c r="AX16" t="s">
         <v>34</v>
       </c>
+      <c r="AY16" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3005,8 +3044,11 @@
       <c r="AX17" t="s">
         <v>35</v>
       </c>
+      <c r="AY17" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3151,8 +3193,11 @@
       <c r="AX18" t="s">
         <v>35</v>
       </c>
+      <c r="AY18" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3297,8 +3342,11 @@
       <c r="AX19" t="s">
         <v>35</v>
       </c>
+      <c r="AY19" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3443,8 +3491,11 @@
       <c r="AX20" t="s">
         <v>35</v>
       </c>
+      <c r="AY20" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3589,8 +3640,11 @@
       <c r="AX21" t="s">
         <v>35</v>
       </c>
+      <c r="AY21" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3735,8 +3789,11 @@
       <c r="AX22" t="s">
         <v>35</v>
       </c>
+      <c r="AY22" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3881,8 +3938,11 @@
       <c r="AX23" t="s">
         <v>35</v>
       </c>
+      <c r="AY23" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -4027,8 +4087,11 @@
       <c r="AX24" t="s">
         <v>35</v>
       </c>
+      <c r="AY24" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -4173,8 +4236,11 @@
       <c r="AX25" t="s">
         <v>35</v>
       </c>
+      <c r="AY25" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -4319,8 +4385,11 @@
       <c r="AX26" t="s">
         <v>35</v>
       </c>
+      <c r="AY26" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -4465,8 +4534,11 @@
       <c r="AX27" t="s">
         <v>35</v>
       </c>
+      <c r="AY27" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -4611,8 +4683,11 @@
       <c r="AX28" t="s">
         <v>35</v>
       </c>
+      <c r="AY28" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -4757,8 +4832,11 @@
       <c r="AX29" t="s">
         <v>35</v>
       </c>
+      <c r="AY29" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -4902,6 +4980,9 @@
       </c>
       <c r="AX30" t="s">
         <v>34</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aula 07 - INDMO
</commit_message>
<xml_diff>
--- a/2des/chamada.xlsx
+++ b/2des/chamada.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2022\2des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419AA9BB-4DAF-4CC4-91B3-8121721BA9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD54860E-4ED9-40B5-96C4-8BE30F77D55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="37">
   <si>
     <t>Aluno</t>
   </si>
@@ -188,8 +188,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BB24" sqref="BB24"/>
+      <selection pane="topRight" activeCell="BD29" sqref="BD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +546,7 @@
     <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="55" width="7" customWidth="1"/>
+    <col min="56" max="65" width="7" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
@@ -699,7 +700,7 @@
       <c r="AZ1" s="2">
         <v>44831</v>
       </c>
-      <c r="BA1" s="4">
+      <c r="BA1" s="2">
         <v>44832</v>
       </c>
       <c r="BB1" s="2">
@@ -708,34 +709,34 @@
       <c r="BC1" s="2">
         <v>44834</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="BD1" s="2">
         <v>44837</v>
       </c>
-      <c r="BE1" s="1">
+      <c r="BE1" s="2">
         <v>44838</v>
       </c>
-      <c r="BF1" s="1">
+      <c r="BF1" s="2">
         <v>44839</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="BG1" s="2">
         <v>44840</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="BH1" s="2">
         <v>44841</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="BI1" s="2">
         <v>44844</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BJ1" s="2">
         <v>44845</v>
       </c>
-      <c r="BK1" s="1">
+      <c r="BK1" s="2">
         <v>44846</v>
       </c>
-      <c r="BL1" s="1">
+      <c r="BL1" s="2">
         <v>44847</v>
       </c>
-      <c r="BM1" s="1">
+      <c r="BM1" s="2">
         <v>44848</v>
       </c>
     </row>
@@ -1099,6 +1100,12 @@
       <c r="BB3" t="s">
         <v>34</v>
       </c>
+      <c r="BC3" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD3" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1263,6 +1270,12 @@
       <c r="BB4" t="s">
         <v>34</v>
       </c>
+      <c r="BC4" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD4" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1427,6 +1440,12 @@
       <c r="BB5" t="s">
         <v>35</v>
       </c>
+      <c r="BC5" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1591,6 +1610,12 @@
       <c r="BB6" t="s">
         <v>35</v>
       </c>
+      <c r="BC6" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1755,6 +1780,12 @@
       <c r="BB7" t="s">
         <v>34</v>
       </c>
+      <c r="BC7" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD7" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1919,6 +1950,12 @@
       <c r="BB8" t="s">
         <v>35</v>
       </c>
+      <c r="BC8" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD8" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2083,6 +2120,12 @@
       <c r="BB9" t="s">
         <v>35</v>
       </c>
+      <c r="BC9" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD9" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2247,6 +2290,12 @@
       <c r="BB10" t="s">
         <v>35</v>
       </c>
+      <c r="BC10" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD10" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2411,6 +2460,12 @@
       <c r="BB11" t="s">
         <v>35</v>
       </c>
+      <c r="BC11" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD11" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2575,6 +2630,12 @@
       <c r="BB12" t="s">
         <v>35</v>
       </c>
+      <c r="BC12" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD12" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2828,6 +2889,12 @@
       <c r="BB14" t="s">
         <v>35</v>
       </c>
+      <c r="BC14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD14" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2992,6 +3059,12 @@
       <c r="BB15" t="s">
         <v>35</v>
       </c>
+      <c r="BC15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD15" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3156,8 +3229,14 @@
       <c r="BB16" t="s">
         <v>35</v>
       </c>
+      <c r="BC16" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD16" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3320,8 +3399,14 @@
       <c r="BB17" t="s">
         <v>35</v>
       </c>
+      <c r="BC17" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD17" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3484,8 +3569,14 @@
       <c r="BB18" t="s">
         <v>35</v>
       </c>
+      <c r="BC18" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD18" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3648,8 +3739,14 @@
       <c r="BB19" t="s">
         <v>35</v>
       </c>
+      <c r="BC19" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD19" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3812,8 +3909,14 @@
       <c r="BB20" t="s">
         <v>35</v>
       </c>
+      <c r="BC20" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD20" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3976,8 +4079,14 @@
       <c r="BB21" t="s">
         <v>35</v>
       </c>
+      <c r="BC21" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD21" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -4140,8 +4249,14 @@
       <c r="BB22" t="s">
         <v>34</v>
       </c>
+      <c r="BC22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD22" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -4304,8 +4419,14 @@
       <c r="BB23" t="s">
         <v>35</v>
       </c>
+      <c r="BC23" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD23" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -4468,8 +4589,14 @@
       <c r="BB24" t="s">
         <v>35</v>
       </c>
+      <c r="BC24" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD24" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -4632,8 +4759,14 @@
       <c r="BB25" t="s">
         <v>35</v>
       </c>
+      <c r="BC25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD25" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -4796,8 +4929,14 @@
       <c r="BB26" t="s">
         <v>35</v>
       </c>
+      <c r="BC26" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD26" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -4960,8 +5099,14 @@
       <c r="BB27" t="s">
         <v>35</v>
       </c>
+      <c r="BC27" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD27" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -5124,8 +5269,14 @@
       <c r="BB28" t="s">
         <v>34</v>
       </c>
+      <c r="BC28" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD28" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -5288,8 +5439,14 @@
       <c r="BB29" t="s">
         <v>35</v>
       </c>
+      <c r="BC29" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD29" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -5450,6 +5607,12 @@
         <v>35</v>
       </c>
       <c r="BB30" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC30" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD30" s="4" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2des pwbe aulas12 e 13
</commit_message>
<xml_diff>
--- a/2des/chamada.xlsx
+++ b/2des/chamada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2022\2des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E8CB12-672D-438D-994D-BC22FD6D7DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA02815-A7EF-4DB7-B5FF-8F4DAA7CB60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="37">
   <si>
     <t>Aluno</t>
   </si>
@@ -525,7 +525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CA26" sqref="CA26"/>
+      <selection pane="topRight" activeCell="CB26" sqref="CB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,6 +1311,9 @@
       <c r="CA3" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="CB3" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1547,6 +1550,9 @@
       <c r="CA4" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB4" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1783,6 +1789,9 @@
       <c r="CA5" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="CB5" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2019,6 +2028,9 @@
       <c r="CA6" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2255,6 +2267,9 @@
       <c r="CA7" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB7" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2491,6 +2506,9 @@
       <c r="CA8" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB8" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2727,6 +2745,9 @@
       <c r="CA9" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB9" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2963,6 +2984,9 @@
       <c r="CA10" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB10" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3199,6 +3223,9 @@
       <c r="CA11" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB11" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3435,6 +3462,9 @@
       <c r="CA12" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB12" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3763,6 +3793,9 @@
       <c r="CA14" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB14" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3999,6 +4032,9 @@
       <c r="CA15" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="CB15" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4235,8 +4271,11 @@
       <c r="CA16" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB16" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4471,8 +4510,11 @@
       <c r="CA17" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB17" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="18" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -4707,8 +4749,11 @@
       <c r="CA18" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB18" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="19" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -4943,8 +4988,11 @@
       <c r="CA19" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB19" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="20" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -5179,8 +5227,11 @@
       <c r="CA20" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB20" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="21" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -5415,8 +5466,11 @@
       <c r="CA21" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB21" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="22" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -5651,8 +5705,11 @@
       <c r="CA22" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB22" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="23" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -5887,8 +5944,11 @@
       <c r="CA23" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB23" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="24" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -6123,8 +6183,11 @@
       <c r="CA24" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="CB24" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="25" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -6359,8 +6422,11 @@
       <c r="CA25" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB25" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="26" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -6595,8 +6661,11 @@
       <c r="CA26" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB26" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="27" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -6831,8 +6900,11 @@
       <c r="CA27" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB27" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="28" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -7067,8 +7139,11 @@
       <c r="CA28" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB28" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="29" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -7303,8 +7378,11 @@
       <c r="CA29" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="CB29" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="30" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -7537,6 +7615,9 @@
         <v>35</v>
       </c>
       <c r="CA30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="CB30" s="4" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>